<commit_message>
update WS Liste und Commit der Postman collection
</commit_message>
<xml_diff>
--- a/SYP(MUH)/WebServices_Liste.xlsx
+++ b/SYP(MUH)/WebServices_Liste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Sonnek\Desktop\5. Klasse\Travel_Project\github\TravelAdvisor\SYP(MUH)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3CED46-A41D-4A58-A389-5803346117FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5543BD83-801C-49F3-9706-A26AE57C7D65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Branchen" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
   <si>
     <t>WebServices</t>
   </si>
@@ -381,6 +381,12 @@
       </rPr>
       <t>wird ein Wert nicht gesetzt, bleibt der alte bestehen</t>
     </r>
+  </si>
+  <si>
+    <t>gibt Location des übergebenen Besitzers zurück</t>
+  </si>
+  <si>
+    <t>Gibt Locations im übergebenen Umkreis</t>
   </si>
 </sst>
 </file>
@@ -825,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1054,15 +1060,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A8964C-D9F4-4368-A3F8-12F4D850CEFC}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="68.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="73.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="46.88671875" customWidth="1"/>
@@ -1241,6 +1247,16 @@
       </c>
       <c r="H8" s="4" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C9" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C10" s="12" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug behoben: Updaten von koordinaten jetzt möglich
</commit_message>
<xml_diff>
--- a/SYP(MUH)/WebServices_Liste.xlsx
+++ b/SYP(MUH)/WebServices_Liste.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Sonnek\Desktop\5. Klasse\Travel_Project\github\TravelAdvisor\SYP(MUH)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33F142B-DA0A-4804-99A1-EB755C7F4275}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D11096-7935-42DE-A99F-E72EEA578148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Branchen" sheetId="1" r:id="rId1"/>
     <sheet name="Locations" sheetId="2" r:id="rId2"/>
     <sheet name="Prämien" sheetId="3" r:id="rId3"/>
+    <sheet name="Rezensionen" sheetId="4" r:id="rId4"/>
+    <sheet name="Besuch" sheetId="5" r:id="rId5"/>
+    <sheet name="Praemie_eingeloest" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="72">
   <si>
     <t>WebServices</t>
   </si>
@@ -420,9 +423,6 @@
 "locationId": "UUID"}</t>
   </si>
   <si>
-    <t>Erstellen einer neuen Prämie</t>
-  </si>
-  <si>
     <t>{ 
 "bezeichnung": ,
 "punkte": 100,
@@ -438,6 +438,81 @@
   </si>
   <si>
     <t>Löschen einer Prämie</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/TravelAdvisor_WebServices/TravelGuide/rezensionenList</t>
+  </si>
+  <si>
+    <t>Liste aller Rezensionen</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/TravelAdvisor_WebServices/TravelGuide/rezensionenDetail/:id</t>
+  </si>
+  <si>
+    <t>Details einer einzelnen Rezension</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/TravelAdvisor_WebServices/TravelGuide/rezensionenDetail</t>
+  </si>
+  <si>
+    <t>{
+		"locationid": "5e010350-72a3-4435-8455-17f4e9f3ff66",
+		"besucherid": "350e7145-5f8d-4203-94e0-8aa6e208c73f",
+		"bewertung": 4
+	}</t>
+  </si>
+  <si>
+    <t>Erstellen einer neuen Rezension</t>
+  </si>
+  <si>
+    <t>{
+    "besucherid": "350e7145-5f8d-4203-94e0-8aa6e208c73f",
+    "bewertung": 4,
+    "id": "9e71af73-2e47-412d-9e89-6b90d7bf7956",
+    "locationid": "5e010350-72a3-4435-8455-17f4e9f3ff66",
+    "timestamp": "2019-11-14T14:33:21.917Z[UTC]"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "bewertung": 5
+}</t>
+  </si>
+  <si>
+    <t>{
+    "besucherid": "350e7145-5f8d-4203-94e0-8aa6e208c73f",
+    "bewertung": 5,
+    "id": "9e71af73-2e47-412d-9e89-6b90d7bf7956",
+    "locationid": "5e010350-72a3-4435-8455-17f4e9f3ff66",
+    "timestamp": "2019-11-14T14:40:32.709Z[UTC]"
+}</t>
+  </si>
+  <si>
+    <t>Löschen einer Rezension</t>
+  </si>
+  <si>
+    <t>400, 404</t>
+  </si>
+  <si>
+    <t>[
+{
+    "besucherid": "350e7145-5f8d-4203-94e0-8aa6e208c73f",
+    "bewertung": 4,
+    "id": "9e71af73-2e47-412d-9e89-6b90d7bf7956",
+    "locationid": "5e010350-72a3-4435-8455-17f4e9f3ff66",
+    "timestamp": "2019-11-14T14:33:21.917Z[UTC]"
+}
+, … 
+]</t>
+  </si>
+  <si>
+    <t>Updaten einer bestehenden Rezension. 
+Bemerkung: Nur ein Updaten der Bewertung (1-5) möglich, bewertung muss übergeben werden
+funktioniert, Fehlermeldungen aber nicht ideal</t>
+  </si>
+  <si>
+    <t>Erstellen einer neuen Prämie, 
+(Erstellen einer Prämie mit der Bezeichnung "" möglich)</t>
   </si>
 </sst>
 </file>
@@ -499,7 +574,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -509,6 +584,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -526,7 +613,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -559,14 +646,23 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -886,7 +982,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:I6"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -902,27 +998,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
       <c r="G1" s="9"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
@@ -939,14 +1035,14 @@
       <c r="D3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15" t="s">
+      <c r="F3" s="16"/>
+      <c r="G3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="15"/>
+      <c r="H3" s="16"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E4" s="4" t="s">
@@ -1116,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A8964C-D9F4-4368-A3F8-12F4D850CEFC}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1133,14 +1229,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1156,14 +1252,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15" t="s">
+      <c r="F2" s="16"/>
+      <c r="G2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="15"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
@@ -1335,8 +1431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A9BAA7-38F1-46B8-B89D-A5F77F709C66}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1350,16 +1446,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -1374,14 +1470,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15" t="s">
+      <c r="F2" s="16"/>
+      <c r="G2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="15"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
@@ -1402,13 +1498,13 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="14" t="s">
         <v>46</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="17" t="s">
         <v>49</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -1428,13 +1524,13 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="14" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="17" t="s">
         <v>50</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1454,17 +1550,17 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="14" t="s">
         <v>48</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>53</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>54</v>
       </c>
       <c r="E6" s="4">
         <v>201</v>
@@ -1480,17 +1576,17 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="14" t="s">
         <v>47</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>55</v>
+      <c r="C7" s="17" t="s">
+        <v>54</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" s="4">
         <v>200</v>
@@ -1499,21 +1595,21 @@
         <v>52</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>47</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>57</v>
+      <c r="C8" s="17" t="s">
+        <v>56</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>8</v>
@@ -1557,4 +1653,245 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId6"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C798FB6-B3FD-4DC1-B375-2CBAA26E1863}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="71.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.21875" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="4" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="4">
+        <v>200</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="4" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4">
+        <v>200</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="4">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="4" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="4">
+        <v>201</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="4">
+        <v>400</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="4" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="4">
+        <v>200</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="4">
+        <v>204</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="4">
+        <v>404</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{398794AA-EA72-4171-BFFB-966B54F5B353}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{76BD7064-3D10-4D30-90A7-046DE002C809}"/>
+    <hyperlink ref="A6" r:id="rId3" xr:uid="{F44E83B7-D637-48B3-93C8-12304602CF3F}"/>
+    <hyperlink ref="A8" r:id="rId4" xr:uid="{C45B1E8F-E0EF-4DC3-86B6-C47F8F001193}"/>
+    <hyperlink ref="A7" r:id="rId5" xr:uid="{E9C0E1EB-9731-46CC-9140-CF2AEAF65591}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F27C790-F70C-4477-A3BD-8A314CB8EACD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57455783-080B-44C4-A19C-B76904128682}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Performantere Lösung beim Laden der Locations, Distanzberechnung genauer
</commit_message>
<xml_diff>
--- a/SYP(MUH)/WebServices_Liste.xlsx
+++ b/SYP(MUH)/WebServices_Liste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Sonnek\Desktop\5. Klasse\Travel_Project\github\TravelAdvisor\SYP(MUH)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D11096-7935-42DE-A99F-E72EEA578148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600BEF8B-7A01-406C-84EE-4377CD36FAD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Branchen" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="78">
   <si>
     <t>WebServices</t>
   </si>
@@ -390,9 +390,6 @@
     <t>gibt Location des übergebenen Besitzers zurück</t>
   </si>
   <si>
-    <t>Gibt Locations im übergebenen Umkreis</t>
-  </si>
-  <si>
     <t>http://localhost:8080/TravelAdvisor_WebServices/TravelGuide/praemienList</t>
   </si>
   <si>
@@ -513,6 +510,32 @@
   <si>
     <t>Erstellen einer neuen Prämie, 
 (Erstellen einer Prämie mit der Bezeichnung "" möglich)</t>
+  </si>
+  <si>
+    <t>Queryparameter:
+"distanz": Distanz in m
+"x": X-GeoKoordinate
+"y": Y-GeoKoordinate
+"loadBranchen": boolean ob Branchen mitgeladen werden sollen (Standard: false)</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/TravelAdvisor_WebServices/TravelGuide/locationDetail/:id/branchen</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/TravelAdvisor_WebServices/TravelGuide/locationDetail/:id/praemien</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/TravelAdvisor_WebServices/TravelGuide/locationDetail/:id/rezensionen</t>
+  </si>
+  <si>
+    <t>Gibt die Branchen
+einer Location zurück</t>
+  </si>
+  <si>
+    <t>Gibt alle Prämien einer Location zurück</t>
+  </si>
+  <si>
+    <t>Gibt alle Rezensionen einer Location zurück</t>
   </si>
 </sst>
 </file>
@@ -649,12 +672,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -663,6 +680,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -998,27 +1021,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
       <c r="G1" s="9"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
@@ -1035,14 +1058,14 @@
       <c r="D3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16" t="s">
+      <c r="F3" s="19"/>
+      <c r="G3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="16"/>
+      <c r="H3" s="19"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E4" s="4" t="s">
@@ -1210,15 +1233,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A8964C-D9F4-4368-A3F8-12F4D850CEFC}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="73.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="83.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="46.88671875" customWidth="1"/>
@@ -1229,14 +1252,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1252,14 +1275,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="16"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
@@ -1288,8 +1311,8 @@
       <c r="C4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>8</v>
+      <c r="D4" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="E4" s="4">
         <v>200</v>
@@ -1297,8 +1320,8 @@
       <c r="F4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="4">
-        <v>404</v>
+      <c r="G4" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>8</v>
@@ -1403,10 +1426,77 @@
       <c r="C9" s="12" t="s">
         <v>44</v>
       </c>
+      <c r="D9" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="C10" s="12" t="s">
-        <v>45</v>
+        <v>75</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="4">
+        <v>200</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="4">
+        <v>200</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="4">
+        <v>200</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1421,9 +1511,12 @@
     <hyperlink ref="A6" r:id="rId3" xr:uid="{75104C59-5384-4A7A-BE91-F02B6511DCEC}"/>
     <hyperlink ref="A7" r:id="rId4" xr:uid="{4226BD69-CDE2-43AB-B4F9-C98B5A6F454A}"/>
     <hyperlink ref="A8" r:id="rId5" xr:uid="{E1822124-8C1C-41F6-A5B6-336590251216}"/>
+    <hyperlink ref="A10" r:id="rId6" xr:uid="{B0588D0A-7251-4EBE-B491-88203AF7ACAA}"/>
+    <hyperlink ref="A11" r:id="rId7" xr:uid="{48FF3EA8-AC01-459A-B3AB-F19641DDB3A0}"/>
+    <hyperlink ref="A12" r:id="rId8" xr:uid="{40114E0B-68B3-45BE-9AD7-272361B7B2CC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -1446,16 +1539,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -1470,14 +1563,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="16"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
@@ -1499,13 +1592,13 @@
     </row>
     <row r="4" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>49</v>
+      <c r="C4" s="15" t="s">
+        <v>48</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>8</v>
@@ -1514,7 +1607,7 @@
         <v>200</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>8</v>
@@ -1525,13 +1618,13 @@
     </row>
     <row r="5" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>50</v>
+      <c r="C5" s="15" t="s">
+        <v>49</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>8</v>
@@ -1540,7 +1633,7 @@
         <v>200</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G5" s="4">
         <v>404</v>
@@ -1551,22 +1644,22 @@
     </row>
     <row r="6" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="19" t="s">
-        <v>71</v>
+      <c r="C6" s="17" t="s">
+        <v>70</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E6" s="4">
         <v>201</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G6" s="4">
         <v>400</v>
@@ -1577,25 +1670,25 @@
     </row>
     <row r="7" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>54</v>
+      <c r="C7" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E7" s="4">
         <v>200</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>8</v>
@@ -1603,13 +1696,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>56</v>
+      <c r="C8" s="15" t="s">
+        <v>55</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>8</v>
@@ -1676,16 +1769,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -1700,14 +1793,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="16"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E3" s="4" t="s">
@@ -1725,13 +1818,13 @@
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>58</v>
+      <c r="C4" s="15" t="s">
+        <v>57</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>8</v>
@@ -1740,7 +1833,7 @@
         <v>200</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>8</v>
@@ -1751,13 +1844,13 @@
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>60</v>
+      <c r="C5" s="15" t="s">
+        <v>59</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>8</v>
@@ -1766,7 +1859,7 @@
         <v>200</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G5" s="4">
         <v>404</v>
@@ -1774,22 +1867,22 @@
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>63</v>
+      <c r="C6" s="15" t="s">
+        <v>62</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E6" s="4">
         <v>201</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G6" s="4">
         <v>400</v>
@@ -1800,25 +1893,25 @@
     </row>
     <row r="7" spans="1:8" s="4" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>70</v>
+      <c r="C7" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" s="4">
         <v>200</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>8</v>
@@ -1826,13 +1919,13 @@
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>67</v>
+      <c r="C8" s="15" t="s">
+        <v>66</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>8</v>
@@ -1886,7 +1979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57455783-080B-44C4-A19C-B76904128682}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Usermanagement in der WebApp implementiert
</commit_message>
<xml_diff>
--- a/SYP(MUH)/WebServices_Liste.xlsx
+++ b/SYP(MUH)/WebServices_Liste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Sonnek\Desktop\5. Klasse\Travel_Project\github\TravelAdvisor\SYP(MUH)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600BEF8B-7A01-406C-84EE-4377CD36FAD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA54B07-C2A2-49FB-B7B7-5A079AC0110F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Branchen" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="89">
   <si>
     <t>WebServices</t>
   </si>
@@ -537,6 +537,57 @@
   <si>
     <t>Gibt alle Rezensionen einer Location zurück</t>
   </si>
+  <si>
+    <t>Einfügen eines Besuchs
+ einer Location</t>
+  </si>
+  <si>
+    <t>{
+locationId: "…",
+besucherId: "…"
+}</t>
+  </si>
+  <si>
+    <t>[ {
+"id": "asdf"
+"Resource1": URL, 
+"Resource2": URL,
+"from": ,
+"to":
+}, ….]</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/TravelAdvisor_WebServices/TravelGuide/besuche</t>
+  </si>
+  <si>
+    <t>/besuche/:bid</t>
+  </si>
+  <si>
+    <t>Besuch löschen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liefert bestimmten Besuch zurück
+</t>
+  </si>
+  <si>
+    <t>{
+"id": "asdf"
+"location": URL, 
+"besucher": URL
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liefert alle Besuche zurück
+</t>
+  </si>
+  <si>
+    <t>/besuche</t>
+  </si>
+  <si>
+    <t>QueryParams:
+locationId; 
+besucherId;</t>
+  </si>
 </sst>
 </file>
 
@@ -597,7 +648,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -622,6 +673,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -636,7 +693,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -686,6 +743,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1235,8 +1298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A8964C-D9F4-4368-A3F8-12F4D850CEFC}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1752,8 +1815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C798FB6-B3FD-4DC1-B375-2CBAA26E1863}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection sqref="A1:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1965,12 +2028,184 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F27C790-F70C-4477-A3BD-8A314CB8EACD}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="66.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.21875" customWidth="1"/>
+    <col min="7" max="7" width="17.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="19"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="4">
+        <v>200</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="8">
+        <v>204</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="8">
+        <v>404</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="8">
+        <v>200</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="8">
+        <v>200</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{69BF3115-3046-423F-91C5-5D9E1A57EB02}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1980,7 +2215,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Einfügen der Webservice-Liste in die Abgabe
</commit_message>
<xml_diff>
--- a/SYP(MUH)/WebServices_Liste.xlsx
+++ b/SYP(MUH)/WebServices_Liste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Sonnek\Desktop\5. Klasse\Travel_Project\github\TravelAdvisor\SYP(MUH)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689F55D6-7AB9-4879-86FB-3A183AF02A23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1ED2FB2-EB3D-4936-9421-895D6EB92546}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Branchen" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="101">
   <si>
     <t>WebServices</t>
   </si>
@@ -534,9 +534,6 @@
     <t>http://localhost:8080/TravelAdvisor_WebServices/TravelGuide/besuche</t>
   </si>
   <si>
-    <t>/besuche/:bid</t>
-  </si>
-  <si>
     <t>Besuch löschen</t>
   </si>
   <si>
@@ -553,9 +550,6 @@
   <si>
     <t xml:space="preserve">Liefert alle Besuche zurück
 </t>
-  </si>
-  <si>
-    <t>/besuche</t>
   </si>
   <si>
     <t>QueryParams:
@@ -631,12 +625,21 @@
   <si>
     <t>id als QueryParameter</t>
   </si>
+  <si>
+    <t>Prämien</t>
+  </si>
+  <si>
+    <t>Besuch</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/TravelAdvisor_WebServices/TravelGuide/besuche/:bid</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -690,19 +693,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -736,7 +740,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -768,21 +772,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -790,14 +802,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1116,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1133,27 +1140,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
       <c r="G1" s="9"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
@@ -1170,14 +1177,14 @@
       <c r="D3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20" t="s">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="20"/>
+      <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E4" s="4" t="s">
@@ -1193,14 +1200,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="24" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1218,7 +1225,7 @@
       <c r="H5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="13"/>
+      <c r="I5" s="23"/>
     </row>
     <row r="6" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
@@ -1227,7 +1234,7 @@
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -1245,7 +1252,7 @@
       <c r="H6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="13"/>
+      <c r="I6" s="23"/>
     </row>
     <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
@@ -1254,7 +1261,7 @@
       <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="18" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -1280,7 +1287,7 @@
       <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="18" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="6" t="s">
@@ -1306,7 +1313,7 @@
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="18" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -1347,8 +1354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A8964C-D9F4-4368-A3F8-12F4D850CEFC}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D12" sqref="D4:D12"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1364,14 +1371,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1387,14 +1394,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20" t="s">
+      <c r="F2" s="22"/>
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="20"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
@@ -1423,8 +1430,8 @@
       <c r="C4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="21" t="s">
-        <v>84</v>
+      <c r="D4" s="18" t="s">
+        <v>82</v>
       </c>
       <c r="E4" s="4">
         <v>200</v>
@@ -1449,7 +1456,7 @@
       <c r="C5" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="19" t="s">
         <v>33</v>
       </c>
       <c r="E5" s="4">
@@ -1475,7 +1482,7 @@
       <c r="C6" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="19" t="s">
         <v>38</v>
       </c>
       <c r="E6" s="4">
@@ -1501,11 +1508,20 @@
       <c r="C7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="20" t="s">
         <v>39</v>
       </c>
       <c r="E7" s="4">
         <v>204</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>404</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="288" x14ac:dyDescent="0.3">
@@ -1518,7 +1534,7 @@
       <c r="C8" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="20" t="s">
         <v>39</v>
       </c>
       <c r="E8" s="4">
@@ -1536,7 +1552,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C9" s="12"/>
-      <c r="D9" s="23"/>
+      <c r="D9" s="20"/>
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
@@ -1548,7 +1564,7 @@
       <c r="C10" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="20" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="4">
@@ -1571,7 +1587,7 @@
       <c r="C11" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="20" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="4">
@@ -1594,7 +1610,7 @@
       <c r="C12" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="20" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="4">
@@ -1632,8 +1648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A9BAA7-38F1-46B8-B89D-A5F77F709C66}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1647,16 +1663,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="A1" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -1671,14 +1687,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20" t="s">
+      <c r="F2" s="22"/>
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="20"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
@@ -1699,13 +1715,13 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>44</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>47</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -1725,13 +1741,13 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>48</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1751,13 +1767,13 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>46</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="15" t="s">
         <v>66</v>
       </c>
       <c r="D6" s="12" t="s">
@@ -1777,13 +1793,13 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>52</v>
       </c>
       <c r="D7" s="12" t="s">
@@ -1803,13 +1819,13 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>54</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -1860,8 +1876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C798FB6-B3FD-4DC1-B375-2CBAA26E1863}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1877,16 +1893,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="A1" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -1901,14 +1917,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20" t="s">
+      <c r="F2" s="22"/>
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="20"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E3" s="4" t="s">
@@ -1925,13 +1941,13 @@
       </c>
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" ht="144" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>55</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>56</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -1951,13 +1967,13 @@
       </c>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>57</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>58</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1974,17 +1990,17 @@
       </c>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>59</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>60</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E6" s="4">
         <v>201</v>
@@ -2000,17 +2016,17 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="4" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>57</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>85</v>
+      <c r="C7" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E7" s="4">
         <v>200</v>
@@ -2026,13 +2042,13 @@
       </c>
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>57</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>63</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -2076,7 +2092,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2089,16 +2105,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="A1" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -2113,14 +2129,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20" t="s">
+      <c r="F2" s="22"/>
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="20"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
@@ -2141,13 +2157,13 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>76</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>73</v>
       </c>
       <c r="D4" s="6" t="s">
@@ -2165,14 +2181,14 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>77</v>
+      <c r="A5" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>8</v>
@@ -2191,14 +2207,14 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>77</v>
+      <c r="A6" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>8</v>
@@ -2210,24 +2226,24 @@
         <v>8</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>82</v>
+      <c r="A7" s="13" t="s">
+        <v>76</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>81</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>83</v>
       </c>
       <c r="E7" s="8">
         <v>200</v>
@@ -2250,6 +2266,9 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1" xr:uid="{69BF3115-3046-423F-91C5-5D9E1A57EB02}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{BB033ABE-A4DC-4394-88F3-40E3271EBC51}"/>
+    <hyperlink ref="A6" r:id="rId3" xr:uid="{5E0D696A-FDB7-4688-92E7-0A80BC470435}"/>
+    <hyperlink ref="A7" r:id="rId4" xr:uid="{79F6CE05-FA49-453F-AA70-140A188E01E6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2259,8 +2278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ACE98E0-FE61-4B33-88C0-8470327AEE72}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2275,16 +2294,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="A1" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -2299,14 +2318,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20" t="s">
+      <c r="F2" s="22"/>
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="20"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E3" s="4" t="s">
@@ -2323,14 +2342,14 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>8</v>
@@ -2339,27 +2358,27 @@
         <v>200</v>
       </c>
       <c r="F5" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="B6" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>96</v>
       </c>
       <c r="E6" s="4">
         <v>201</v>
@@ -2375,23 +2394,23 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="E7" s="4">
         <v>204</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G7" s="4">
         <v>404</v>
@@ -2550,7 +2569,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
aktualisieren der WebService-Liste & einfügen von fehlenden CRUD Operationen für den LocationBesuch
</commit_message>
<xml_diff>
--- a/SYP(MUH)/WebServices_Liste.xlsx
+++ b/SYP(MUH)/WebServices_Liste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Sonnek\Desktop\5. Klasse\Travel_Project\github\TravelAdvisor\SYP(MUH)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1ED2FB2-EB3D-4936-9421-895D6EB92546}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5569D7C-6A2C-4973-81CA-8B3EC17F4D06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Branchen" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Rezensionen" sheetId="4" r:id="rId4"/>
     <sheet name="Besuch" sheetId="5" r:id="rId5"/>
     <sheet name="Besitzer" sheetId="7" r:id="rId6"/>
-    <sheet name="Praemie_eingeloest" sheetId="6" r:id="rId7"/>
+    <sheet name="Besucher" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="109">
   <si>
     <t>WebServices</t>
   </si>
@@ -531,9 +531,6 @@
 }, ….]</t>
   </si>
   <si>
-    <t>http://localhost:8080/TravelAdvisor_WebServices/TravelGuide/besuche</t>
-  </si>
-  <si>
     <t>Besuch löschen</t>
   </si>
   <si>
@@ -632,7 +629,48 @@
     <t>Besuch</t>
   </si>
   <si>
-    <t>http://localhost:8080/TravelAdvisor_WebServices/TravelGuide/besuche/:bid</t>
+    <t>http://localhost:8080/TravelAdvisor_WebServices/TravelGuide/locationBesuchDetail</t>
+  </si>
+  <si>
+    <t>{
+besucherId: "..",
+id: "…",
+locationId: "…"
+zeitpunkt: timestamp
+}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/TravelAdvisor_WebServices/TravelGuide/locationBesuchDetail/:id_besuch</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/TravelAdvisor_WebServices/TravelGuide/besucheList</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/TravelAdvisor_WebServices/TravelGuide/besucherDetail/verlauf/:id_besucher</t>
+  </si>
+  <si>
+    <t>Verlauf aller Punkte-Aktionen (einlösen &amp; erhalten) mit jeweiligem Timestamp eines Besuchers</t>
+  </si>
+  <si>
+    <t>{
+id_besucher: "..",
+aktionen: [ {
+"beschreibung": "aktion eingelöst: Biker`s week -30% upd",
+            "punkte": -100,
+            "zeitpunkt": "Mar 22, 2020, 1:11:20 AM",
+            "location": "Andiamo" }, ...
+…]
+}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/TravelAdvisor_WebServices/TravelGuide/besucherDetail/:id_besucher/punkte</t>
+  </si>
+  <si>
+    <t>Liefert die Anzahl der Punkte zurück, 
+die der Benutzer mit der jeweiligen ID gerade hat</t>
+  </si>
+  <si>
+    <t>Integer Zahl</t>
   </si>
 </sst>
 </file>
@@ -796,15 +834,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1123,7 +1161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -1140,27 +1178,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
       <c r="G1" s="9"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
@@ -1177,14 +1215,14 @@
       <c r="D3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22" t="s">
+      <c r="F3" s="24"/>
+      <c r="G3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="22"/>
+      <c r="H3" s="24"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E4" s="4" t="s">
@@ -1207,7 +1245,7 @@
       <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="22" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1225,7 +1263,7 @@
       <c r="H5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="23"/>
+      <c r="I5" s="21"/>
     </row>
     <row r="6" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
@@ -1252,7 +1290,7 @@
       <c r="H6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="23"/>
+      <c r="I6" s="21"/>
     </row>
     <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
@@ -1371,14 +1409,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1394,14 +1432,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22" t="s">
+      <c r="F2" s="24"/>
+      <c r="G2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="22"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
@@ -1431,7 +1469,7 @@
         <v>31</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E4" s="4">
         <v>200</v>
@@ -1663,16 +1701,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="A1" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -1687,14 +1725,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22" t="s">
+      <c r="F2" s="24"/>
+      <c r="G2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="22"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
@@ -1893,16 +1931,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="A1" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -1917,14 +1955,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22" t="s">
+      <c r="F2" s="24"/>
+      <c r="G2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="22"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E3" s="4" t="s">
@@ -2000,7 +2038,7 @@
         <v>60</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E6" s="4">
         <v>201</v>
@@ -2023,10 +2061,10 @@
         <v>21</v>
       </c>
       <c r="C7" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="E7" s="4">
         <v>200</v>
@@ -2092,29 +2130,30 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="66.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="80.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.109375" customWidth="1"/>
     <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.21875" customWidth="1"/>
+    <col min="6" max="6" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.77734375" customWidth="1"/>
+    <col min="8" max="8" width="23.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="A1" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -2129,14 +2168,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22" t="s">
+      <c r="F2" s="24"/>
+      <c r="G2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="22"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
@@ -2156,9 +2195,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>12</v>
@@ -2172,23 +2211,22 @@
       <c r="E4" s="4">
         <v>200</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F4" s="12" t="s">
+        <v>100</v>
+      </c>
       <c r="G4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>8</v>
@@ -2208,13 +2246,13 @@
     </row>
     <row r="6" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>8</v>
@@ -2226,7 +2264,7 @@
         <v>8</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>8</v>
@@ -2234,16 +2272,16 @@
     </row>
     <row r="7" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>80</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>81</v>
       </c>
       <c r="E7" s="8">
         <v>200</v>
@@ -2294,16 +2332,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="A1" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -2318,14 +2356,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22" t="s">
+      <c r="F2" s="24"/>
+      <c r="G2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="22"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E3" s="4" t="s">
@@ -2343,13 +2381,13 @@
     </row>
     <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>8</v>
@@ -2358,27 +2396,27 @@
         <v>200</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>94</v>
       </c>
       <c r="E6" s="4">
         <v>201</v>
@@ -2395,22 +2433,22 @@
     </row>
     <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E7" s="4">
         <v>204</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G7" s="4">
         <v>404</v>
@@ -2566,14 +2604,116 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57455783-080B-44C4-A19C-B76904128682}">
-  <dimension ref="A1"/>
+  <dimension ref="B3:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="84" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="38.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="24"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="B5" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="4">
+        <v>200</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6">
+        <v>200</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H6">
+        <v>404</v>
+      </c>
+      <c r="I6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{7698D6EE-E8BC-41B3-90E4-28622AA3AD60}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{DB96DECD-A153-4DC0-A239-EA35B129653E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
kleine Änderung WS_Liste+ Logisches Modell verbessert
</commit_message>
<xml_diff>
--- a/SYP(MUH)/WebServices_Liste.xlsx
+++ b/SYP(MUH)/WebServices_Liste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Sonnek\Desktop\5. Klasse\Travel_Project\github\TravelAdvisor\SYP(MUH)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5569D7C-6A2C-4973-81CA-8B3EC17F4D06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E70BBAF-A645-412C-A9BE-99B0D9A59B5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Branchen" sheetId="1" r:id="rId1"/>
@@ -677,7 +677,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -731,13 +731,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -778,7 +771,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -819,9 +812,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -835,9 +825,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1162,7 +1149,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1178,27 +1165,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
       <c r="G1" s="9"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
@@ -1215,14 +1202,14 @@
       <c r="D3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24" t="s">
+      <c r="F3" s="22"/>
+      <c r="G3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="24"/>
+      <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E4" s="4" t="s">
@@ -1238,14 +1225,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1263,7 +1250,7 @@
       <c r="H5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="21"/>
+      <c r="I5" s="20"/>
     </row>
     <row r="6" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
@@ -1272,7 +1259,7 @@
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -1290,7 +1277,7 @@
       <c r="H6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="21"/>
+      <c r="I6" s="20"/>
     </row>
     <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
@@ -1299,7 +1286,7 @@
       <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -1318,14 +1305,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="6" t="s">
@@ -1351,7 +1338,7 @@
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="17" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -1392,8 +1379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A8964C-D9F4-4368-A3F8-12F4D850CEFC}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1409,14 +1396,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1432,14 +1419,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24" t="s">
+      <c r="F2" s="22"/>
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="24"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
@@ -1458,7 +1445,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="346.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>30</v>
       </c>
@@ -1468,7 +1455,7 @@
       <c r="C4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>81</v>
       </c>
       <c r="E4" s="4">
@@ -1494,7 +1481,7 @@
       <c r="C5" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="18" t="s">
         <v>33</v>
       </c>
       <c r="E5" s="4">
@@ -1520,7 +1507,7 @@
       <c r="C6" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>38</v>
       </c>
       <c r="E6" s="4">
@@ -1546,7 +1533,7 @@
       <c r="C7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>39</v>
       </c>
       <c r="E7" s="4">
@@ -1572,7 +1559,7 @@
       <c r="C8" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="19" t="s">
         <v>39</v>
       </c>
       <c r="E8" s="4">
@@ -1590,7 +1577,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C9" s="12"/>
-      <c r="D9" s="20"/>
+      <c r="D9" s="19"/>
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
@@ -1602,7 +1589,7 @@
       <c r="C10" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="4">
@@ -1625,7 +1612,7 @@
       <c r="C11" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="4">
@@ -1648,7 +1635,7 @@
       <c r="C12" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="4">
@@ -1701,16 +1688,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -1725,14 +1712,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24" t="s">
+      <c r="F2" s="22"/>
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="24"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
@@ -1931,16 +1918,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -1955,14 +1942,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24" t="s">
+      <c r="F2" s="22"/>
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="24"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E3" s="4" t="s">
@@ -2130,7 +2117,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C4" sqref="C4:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2144,16 +2131,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -2168,14 +2155,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24" t="s">
+      <c r="F2" s="22"/>
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="24"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
@@ -2202,7 +2189,7 @@
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="17" t="s">
         <v>73</v>
       </c>
       <c r="D4" s="6" t="s">
@@ -2225,7 +2212,7 @@
       <c r="B5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="17" t="s">
         <v>76</v>
       </c>
       <c r="D5" s="8" t="s">
@@ -2251,7 +2238,7 @@
       <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="17" t="s">
         <v>77</v>
       </c>
       <c r="D6" s="8" t="s">
@@ -2277,10 +2264,10 @@
       <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>80</v>
       </c>
       <c r="E7" s="8">
@@ -2332,16 +2319,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -2356,14 +2343,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24" t="s">
+      <c r="F2" s="22"/>
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="24"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E3" s="4" t="s">
@@ -2383,7 +2370,7 @@
       <c r="A5" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="12" t="s">
@@ -2409,7 +2396,7 @@
       <c r="A6" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="12" t="s">
@@ -2435,7 +2422,7 @@
       <c r="A7" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="19" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="12" t="s">
@@ -2606,8 +2593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57455783-080B-44C4-A19C-B76904128682}">
   <dimension ref="B3:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2633,14 +2620,14 @@
       <c r="E3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24" t="s">
+      <c r="G3" s="22"/>
+      <c r="H3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="24"/>
+      <c r="I3" s="22"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>
@@ -2667,7 +2654,7 @@
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="17" t="s">
         <v>104</v>
       </c>
       <c r="E5" s="6"/>
@@ -2688,7 +2675,7 @@
       <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="17" t="s">
         <v>107</v>
       </c>
       <c r="F6">

</xml_diff>

<commit_message>
WebserviceListe formatiert + in Doku aktualisiert und Datenmodelle in Doku eingefügt
</commit_message>
<xml_diff>
--- a/SYP(MUH)/WebServices_Liste.xlsx
+++ b/SYP(MUH)/WebServices_Liste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan Sonnek\Desktop\5. Klasse\Travel_Project\github\TravelAdvisor\SYP(MUH)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E70BBAF-A645-412C-A9BE-99B0D9A59B5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0894DF-3083-445D-8625-88929A237FC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Branchen" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="110">
   <si>
     <t>WebServices</t>
   </si>
@@ -426,9 +426,6 @@
 }</t>
   </si>
   <si>
-    <t>Updaten einer bestehenden Prämie</t>
-  </si>
-  <si>
     <t>404, 400</t>
   </si>
   <si>
@@ -562,10 +559,6 @@
 besitzer: ID des Besitzers nach dem gefiltert werden soll</t>
   </si>
   <si>
-    <t xml:space="preserve">Updaten einer bestehenden Rezension. 
-</t>
-  </si>
-  <si>
     <t>{
     "bewertung": 5,
     "text": "Super!"
@@ -671,6 +664,23 @@
   </si>
   <si>
     <t>Integer Zahl</t>
+  </si>
+  <si>
+    <t>"branchen": [
+        {
+            "bezeichnung": "Gastronomie",
+            "id": "196c207c-9352-4a30-b0db-684b971967ec"
+        }, …..
+    ]</t>
+  </si>
+  <si>
+    <t>Updaten einer bestehenden 
+Prämie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updaten einer bestehenden
+ Rezension. 
+</t>
   </si>
 </sst>
 </file>
@@ -732,18 +742,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -771,7 +775,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -806,25 +810,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1165,27 +1163,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
       <c r="G1" s="9"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
@@ -1202,14 +1200,14 @@
       <c r="D3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22" t="s">
+      <c r="F3" s="20"/>
+      <c r="G3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="22"/>
+      <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E4" s="4" t="s">
@@ -1232,7 +1230,7 @@
       <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1250,7 +1248,7 @@
       <c r="H5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="20"/>
+      <c r="I5" s="18"/>
     </row>
     <row r="6" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
@@ -1259,7 +1257,7 @@
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="15" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -1277,7 +1275,7 @@
       <c r="H6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="20"/>
+      <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
@@ -1286,7 +1284,7 @@
       <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -1312,7 +1310,7 @@
       <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="15" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="6" t="s">
@@ -1338,7 +1336,7 @@
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -1379,8 +1377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A8964C-D9F4-4368-A3F8-12F4D850CEFC}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1396,14 +1394,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1419,14 +1417,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22" t="s">
+      <c r="F2" s="20"/>
+      <c r="G2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="22"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
@@ -1455,8 +1453,8 @@
       <c r="C4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>81</v>
+      <c r="D4" s="15" t="s">
+        <v>80</v>
       </c>
       <c r="E4" s="4">
         <v>200</v>
@@ -1471,7 +1469,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="349.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>32</v>
       </c>
@@ -1481,7 +1479,7 @@
       <c r="C5" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>33</v>
       </c>
       <c r="E5" s="4">
@@ -1507,7 +1505,7 @@
       <c r="C6" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="16" t="s">
         <v>38</v>
       </c>
       <c r="E6" s="4">
@@ -1533,7 +1531,7 @@
       <c r="C7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="17" t="s">
         <v>39</v>
       </c>
       <c r="E7" s="4">
@@ -1559,7 +1557,7 @@
       <c r="C8" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="17" t="s">
         <v>39</v>
       </c>
       <c r="E8" s="4">
@@ -1577,24 +1575,27 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C9" s="12"/>
-      <c r="D9" s="19"/>
-    </row>
-    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D9" s="17"/>
+    </row>
+    <row r="10" spans="1:8" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="17" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="4">
         <v>200</v>
       </c>
+      <c r="F10" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="G10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1602,22 +1603,25 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="17" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="4">
         <v>200</v>
       </c>
+      <c r="F11" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="G11" s="4" t="s">
         <v>8</v>
       </c>
@@ -1625,21 +1629,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="178.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="4">
         <v>200</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>8</v>
@@ -1673,14 +1680,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A9BAA7-38F1-46B8-B89D-A5F77F709C66}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="69.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
     <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.77734375" customWidth="1"/>
     <col min="6" max="6" width="21.6640625" customWidth="1"/>
@@ -1688,16 +1695,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="A1" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -1712,14 +1719,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22" t="s">
+      <c r="F2" s="20"/>
+      <c r="G2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="22"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
@@ -1746,7 +1753,7 @@
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="17" t="s">
         <v>47</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -1772,7 +1779,7 @@
       <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="17" t="s">
         <v>48</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1799,7 +1806,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>51</v>
@@ -1824,8 +1831,8 @@
       <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>52</v>
+      <c r="C7" s="15" t="s">
+        <v>108</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>51</v>
@@ -1837,7 +1844,7 @@
         <v>50</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>8</v>
@@ -1850,8 +1857,8 @@
       <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>54</v>
+      <c r="C8" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>8</v>
@@ -1902,32 +1909,32 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="71.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="77.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="46.21875" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="56" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="A1" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -1942,14 +1949,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22" t="s">
+      <c r="F2" s="20"/>
+      <c r="G2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="22"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E3" s="4" t="s">
@@ -1967,13 +1974,13 @@
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>56</v>
+      <c r="C4" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>8</v>
@@ -1982,7 +1989,7 @@
         <v>200</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>8</v>
@@ -1993,13 +2000,13 @@
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>58</v>
+      <c r="C5" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>8</v>
@@ -2008,7 +2015,7 @@
         <v>200</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G5" s="4">
         <v>404</v>
@@ -2016,22 +2023,22 @@
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>60</v>
+      <c r="C6" s="17" t="s">
+        <v>59</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E6" s="4">
         <v>201</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G6" s="4">
         <v>400</v>
@@ -2042,25 +2049,25 @@
     </row>
     <row r="7" spans="1:8" s="4" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>82</v>
+      <c r="C7" s="15" t="s">
+        <v>109</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E7" s="4">
         <v>200</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>8</v>
@@ -2068,13 +2075,13 @@
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>63</v>
+      <c r="C8" s="17" t="s">
+        <v>62</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>8</v>
@@ -2116,13 +2123,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F27C790-F70C-4477-A3BD-8A314CB8EACD}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C7"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="80.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="84.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.109375" customWidth="1"/>
     <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.21875" bestFit="1" customWidth="1"/>
@@ -2131,16 +2138,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="A1" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -2155,14 +2162,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22" t="s">
+      <c r="F2" s="20"/>
+      <c r="G2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="22"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
@@ -2184,22 +2191,22 @@
     </row>
     <row r="4" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>74</v>
       </c>
       <c r="E4" s="4">
         <v>200</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>8</v>
@@ -2207,13 +2214,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>76</v>
+      <c r="C5" s="15" t="s">
+        <v>75</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>8</v>
@@ -2233,13 +2240,13 @@
     </row>
     <row r="6" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>77</v>
+      <c r="C6" s="15" t="s">
+        <v>76</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>8</v>
@@ -2251,7 +2258,7 @@
         <v>8</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>8</v>
@@ -2259,22 +2266,22 @@
     </row>
     <row r="7" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>79</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>80</v>
       </c>
       <c r="E7" s="8">
         <v>200</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>8</v>
@@ -2304,7 +2311,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2319,16 +2326,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="A1" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -2343,14 +2350,14 @@
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22" t="s">
+      <c r="F2" s="20"/>
+      <c r="G2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="22"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E3" s="4" t="s">
@@ -2368,13 +2375,13 @@
     </row>
     <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>8</v>
@@ -2383,27 +2390,27 @@
         <v>200</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>93</v>
       </c>
       <c r="E6" s="4">
         <v>201</v>
@@ -2420,22 +2427,22 @@
     </row>
     <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="B7" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="E7" s="4">
         <v>204</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G7" s="4">
         <v>404</v>
@@ -2591,114 +2598,125 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57455783-080B-44C4-A19C-B76904128682}">
-  <dimension ref="B3:I6"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="84" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" customWidth="1"/>
-    <col min="7" max="7" width="38.44140625" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="87.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="38.44140625" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="11" t="s">
+    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="20"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="B2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="C2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="E2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22" t="s">
+      <c r="F2" s="20"/>
+      <c r="G2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="22"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
+      <c r="H2" s="20"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="F3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="4">
+        <v>200</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>103</v>
+      </c>
       <c r="G4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="B5" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="4">
+      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5">
         <v>200</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
+      <c r="F5" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="F6">
-        <v>200</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="H6">
+      <c r="G5">
         <v>404</v>
       </c>
-      <c r="I6" t="s">
+      <c r="H5" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
+  <mergeCells count="3">
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{7698D6EE-E8BC-41B3-90E4-28622AA3AD60}"/>
-    <hyperlink ref="B6" r:id="rId2" xr:uid="{DB96DECD-A153-4DC0-A239-EA35B129653E}"/>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{7698D6EE-E8BC-41B3-90E4-28622AA3AD60}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{DB96DECD-A153-4DC0-A239-EA35B129653E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId3"/>

</xml_diff>